<commit_message>
Different part substitution on bom
</commit_message>
<xml_diff>
--- a/BOM_June2022_Ordering.xlsx
+++ b/BOM_June2022_Ordering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\Projects\SW8E-eZ-FET_Lite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D4E395-0EA9-4A90-AEE6-9F52E0928822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DC0207-66B7-43A6-A7F1-8652B20E5155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{55E32EF4-22F0-48EB-BC60-EF439B220CC1}"/>
   </bookViews>
@@ -427,10 +427,10 @@
     <t>Substituted ERJ-P08F2403V</t>
   </si>
   <si>
-    <t>Substitute TLV70033DDCT, available from ti.com</t>
-  </si>
-  <si>
     <t>Not available from mouser; available from ti.com</t>
+  </si>
+  <si>
+    <t>Substituted NCP699SN33T1G</t>
   </si>
 </sst>
 </file>
@@ -615,11 +615,32 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -638,27 +659,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D93EBA-FE0E-4CA2-A0B4-A8686014B4A1}">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,12 +1006,12 @@
       <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="23"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1032,12 +1032,12 @@
       <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="17"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1058,12 +1058,12 @@
       <c r="F3" s="1">
         <v>6</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="20"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="27"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1084,12 +1084,12 @@
       <c r="F4" s="1">
         <v>2</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="26"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1110,12 +1110,12 @@
       <c r="F5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="27" t="s">
+      <c r="H5" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
     </row>
     <row r="6" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -1256,13 +1256,13 @@
       <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
     </row>
     <row r="13" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1283,13 +1283,13 @@
       <c r="F13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1350,14 +1350,14 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1418,14 +1418,14 @@
       <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20"/>
     </row>
     <row r="20" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1446,14 +1446,14 @@
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -1534,14 +1534,14 @@
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
+      <c r="G24" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="25" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1562,14 +1562,14 @@
       <c r="F25" s="4">
         <v>1</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
+      <c r="G25" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
     </row>
     <row r="26" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
@@ -1590,14 +1590,14 @@
       <c r="F26" s="12">
         <v>1</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G26" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">

</xml_diff>